<commit_message>
commited after getting Backend logic working
</commit_message>
<xml_diff>
--- a/uploads/testshare.xlsx
+++ b/uploads/testshare.xlsx
@@ -46,9 +46,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,83 +354,83 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="2">
         <v>1635428</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1634923</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1634785</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>1634780</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>1633690</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>1630863</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>1627494</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>1627246</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>1626285</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>1623504</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="2">
         <v>1626285</v>
       </c>
     </row>

</xml_diff>